<commit_message>
prediccion IPC Y DESEMPLEO
</commit_message>
<xml_diff>
--- a/src/data/INFLACION.xlsx
+++ b/src/data/INFLACION.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juand\OneDrive\Documentos\Proyecto Modelo Codigo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEONARDO ACUÑA\Documents\6 semestre\MyS\Proyecto-Monitoreo\Backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771902CD-2791-411B-A9FA-DA0BB5E202CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7DBDAF-F386-4631-84DB-23EB0133A1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Año(aaaa)-Mes(mm)</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>2018-01</t>
+  </si>
+  <si>
+    <t>2022-10</t>
   </si>
 </sst>
 </file>
@@ -705,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,8 +902,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>202210</v>
+      <c r="A12" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="B12" s="6">
         <v>12.22</v>

</xml_diff>